<commit_message>
Changed so that file names reflect excel values and not excel formulas.
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19920" windowHeight="10320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16950" windowHeight="8880"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
   <si>
     <t>File Name</t>
   </si>
@@ -30,88 +30,55 @@
     <t>Extension</t>
   </si>
   <si>
-    <t>E:/TV&amp;Movies/Anime/[AnimeRG] Shimoneta (A Boring World Where the Concept of Dirty Jokes Doesn't Exist) [UNCENSORED] [BD] [1080p] [x265] [pseudo]</t>
-  </si>
-  <si>
-    <t>torrent</t>
-  </si>
-  <si>
-    <t>.nfo</t>
-  </si>
-  <si>
-    <t>[AnimeRG] Shimoneta - 01 [1080p] [x265] [pseudo]</t>
+    <t>Folder</t>
+  </si>
+  <si>
+    <t>[Daman] Elfen Lied 01 [1280x720_Blu_Ray_Dual_Audio_FLAC][71978425]</t>
   </si>
   <si>
     <t>.mkv</t>
   </si>
   <si>
-    <t>[AnimeRG] Shimoneta - 02 [1080p] [x265] [pseudo]</t>
-  </si>
-  <si>
-    <t>[AnimeRG] Shimoneta - 03 [1080p] [x265] [pseudo]</t>
-  </si>
-  <si>
-    <t>[AnimeRG] Shimoneta - 04 [1080p] [x265] [pseudo]</t>
-  </si>
-  <si>
-    <t>[AnimeRG] Shimoneta - 05 [1080p] [x265] [pseudo]</t>
-  </si>
-  <si>
-    <t>[AnimeRG] Shimoneta - 06 [1080p] [x265] [pseudo]</t>
-  </si>
-  <si>
-    <t>[AnimeRG] Shimoneta - 07 [1080p] [x265] [pseudo]</t>
-  </si>
-  <si>
-    <t>[AnimeRG] Shimoneta - 08 [1080p] [x265] [pseudo]</t>
-  </si>
-  <si>
-    <t>[AnimeRG] Shimoneta - 09 [1080p] [x265] [pseudo]</t>
-  </si>
-  <si>
-    <t>[AnimeRG] Shimoneta - 10 [1080p] [x265] [pseudo]</t>
-  </si>
-  <si>
-    <t>[AnimeRG] Shimoneta - 11 [1080p] [x265] [pseudo]</t>
-  </si>
-  <si>
-    <t>[AnimeRG] Shimoneta - 12 [1080p] [x265] [pseudo]</t>
-  </si>
-  <si>
-    <t>01 - Whom Public Order and Morality Serve?</t>
-  </si>
-  <si>
-    <t>02 - The Mysteries of Pregnancy</t>
-  </si>
-  <si>
-    <t>03 - How to Love Someone</t>
-  </si>
-  <si>
-    <t>05 - For Whom the Dirty Terrorism Benefits?</t>
-  </si>
-  <si>
-    <t>06 - Handmade Warmth!</t>
-  </si>
-  <si>
-    <t>07 - What SOX Created</t>
-  </si>
-  <si>
-    <t>08 - The Devil Blows His Own Trumpet</t>
-  </si>
-  <si>
-    <t>09 - Do Androids Dream of Electric Masseurs?</t>
-  </si>
-  <si>
-    <t>10 - Masturbation Quest</t>
-  </si>
-  <si>
-    <t>11 - Techno Break</t>
-  </si>
-  <si>
-    <t>12 - Dirty Jokes Forever!</t>
-  </si>
-  <si>
-    <t>04 - The Saying Goes Love Is Justice</t>
+    <t>E:/TV&amp;Movies/Anime/[Daman] Elfen Lied</t>
+  </si>
+  <si>
+    <t>[Daman] Elfen Lied 02 [1280x720_Blu_Ray_Dual_Audio_FLAC][1968c90e]</t>
+  </si>
+  <si>
+    <t>[Daman] Elfen Lied 03 [1280x720_Blu_Ray_Dual_Audio_FLAC][85ac8d66]</t>
+  </si>
+  <si>
+    <t>[Daman] Elfen Lied 04 [1280x720_Blu_Ray_Dual_Audio_FLAC][59abc835]</t>
+  </si>
+  <si>
+    <t>[Daman] Elfen Lied 05 [1280x720_Blu_Ray_Dual_Audio_FLAC][33a67a3b]</t>
+  </si>
+  <si>
+    <t>[Daman] Elfen Lied 06 [1280x720_Blu_Ray_Dual_Audio_FLAC][3ef05c2a]</t>
+  </si>
+  <si>
+    <t>[Daman] Elfen Lied 07 [1280x720_Blu_Ray_Dual_Audio_FLAC][5d4c6a5a]</t>
+  </si>
+  <si>
+    <t>[Daman] Elfen Lied 08 [1280x720_Blu_Ray_Dual_Audio_FLAC][a4abbe62]</t>
+  </si>
+  <si>
+    <t>[Daman] Elfen Lied 09 [1280x720_Blu_Ray_Dual_Audio_FLAC][631d7313]</t>
+  </si>
+  <si>
+    <t>[Daman] Elfen Lied 10 [1280x720_Blu_Ray_Dual_Audio_FLAC][c48df422]</t>
+  </si>
+  <si>
+    <t>[Daman] Elfen Lied 11 [1280x720_Blu_Ray_Dual_Audio_FLAC][ba639ab7]</t>
+  </si>
+  <si>
+    <t>[Daman] Elfen Lied 12 [1280x720_Blu_Ray_Dual_Audio_FLAC][e0889607]</t>
+  </si>
+  <si>
+    <t>[Daman] Elfen Lied 13 [1280x720_Blu_Ray_Dual_Audio_FLAC][740bded2]</t>
+  </si>
+  <si>
+    <t>[Daman] Elfen Lied OVA [1280x720_Blu_Ray_FLAC][e82ad193]</t>
   </si>
 </sst>
 </file>
@@ -451,15 +418,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B2" sqref="B2:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -480,140 +447,210 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
+      <c r="B2" t="str">
+        <f>LEFT(A2,21)</f>
+        <v>[Daman] Elfen Lied 01</v>
+      </c>
       <c r="C2" t="s">
         <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
+        <v>7</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B15" si="0">LEFT(A3,21)</f>
+        <v>[Daman] Elfen Lied 02</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>20</v>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>[Daman] Elfen Lied 03</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
-        <v>21</v>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>[Daman] Elfen Lied 04</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
-        <v>30</v>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>[Daman] Elfen Lied 05</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
-        <v>22</v>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>[Daman] Elfen Lied 06</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
-        <v>23</v>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>[Daman] Elfen Lied 07</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
-        <v>24</v>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>[Daman] Elfen Lied 08</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
-        <v>25</v>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>[Daman] Elfen Lied 09</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B11" t="s">
-        <v>26</v>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>[Daman] Elfen Lied 10</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B12" t="s">
-        <v>27</v>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>[Daman] Elfen Lied 11</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="B13" t="s">
-        <v>28</v>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>[Daman] Elfen Lied 12</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B14" t="s">
-        <v>29</v>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>[Daman] Elfen Lied 13</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>[Daman] Elfen Lied OV</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>